<commit_message>
1. New: Add [Field Group Type and Field Widget Management] screen for user to add react plugins. 2. Bugfix.
</commit_message>
<xml_diff>
--- a/django_backend/var/sys/views/core/ScreenDfn-v0.xlsx
+++ b/django_backend/var/sys/views/core/ScreenDfn-v0.xlsx
@@ -1057,7 +1057,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T214"/>
+  <dimension ref="A1:T213"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1309,7 +1309,7 @@
         </is>
       </c>
       <c r="C13" s="12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13" s="8" t="inlineStr">
         <is>
@@ -7258,12 +7258,12 @@
       <c r="C188" s="12" t="inlineStr"/>
       <c r="D188" s="12" t="inlineStr">
         <is>
-          <t>recordsetField</t>
+          <t>dataField</t>
         </is>
       </c>
       <c r="E188" s="12" t="inlineStr">
         <is>
-          <t>Recordset</t>
+          <t>Data</t>
         </is>
       </c>
       <c r="F188" s="12" t="n"/>
@@ -7271,18 +7271,13 @@
       <c r="H188" s="12" t="inlineStr"/>
       <c r="I188" s="12" t="inlineStr">
         <is>
-          <t>ComboBox</t>
-        </is>
-      </c>
-      <c r="J188" s="12" t="inlineStr">
-        <is>
-          <t>dataUrl: getScreenRecordsets
-values: {"value": "id", "display": "recordset_nm"}</t>
-        </is>
-      </c>
+          <t>TextArea</t>
+        </is>
+      </c>
+      <c r="J188" s="12" t="n"/>
       <c r="K188" s="12" t="inlineStr">
         <is>
-          <t>recordset</t>
+          <t>data</t>
         </is>
       </c>
       <c r="L188" s="12" t="n"/>
@@ -7290,7 +7285,7 @@
       <c r="N188" s="12" t="n"/>
       <c r="O188" s="12" t="inlineStr">
         <is>
-          <t>width: 260px;</t>
+          <t>width: 256px;</t>
         </is>
       </c>
       <c r="P188" s="12" t="n"/>
@@ -7299,12 +7294,12 @@
       <c r="C189" s="12" t="inlineStr"/>
       <c r="D189" s="12" t="inlineStr">
         <is>
-          <t>dataField</t>
+          <t>dataUrlField</t>
         </is>
       </c>
       <c r="E189" s="12" t="inlineStr">
         <is>
-          <t>Data</t>
+          <t>DataUrl</t>
         </is>
       </c>
       <c r="F189" s="12" t="n"/>
@@ -7312,13 +7307,13 @@
       <c r="H189" s="12" t="inlineStr"/>
       <c r="I189" s="12" t="inlineStr">
         <is>
-          <t>TextArea</t>
+          <t>TextBox</t>
         </is>
       </c>
       <c r="J189" s="12" t="n"/>
       <c r="K189" s="12" t="inlineStr">
         <is>
-          <t>data</t>
+          <t>dataUrl</t>
         </is>
       </c>
       <c r="L189" s="12" t="n"/>
@@ -7326,7 +7321,7 @@
       <c r="N189" s="12" t="n"/>
       <c r="O189" s="12" t="inlineStr">
         <is>
-          <t>width: 256px;</t>
+          <t>width: 255px;</t>
         </is>
       </c>
       <c r="P189" s="12" t="n"/>
@@ -7335,12 +7330,12 @@
       <c r="C190" s="12" t="inlineStr"/>
       <c r="D190" s="12" t="inlineStr">
         <is>
-          <t>dataUrlField</t>
+          <t>valuesField</t>
         </is>
       </c>
       <c r="E190" s="12" t="inlineStr">
         <is>
-          <t>DataUrl</t>
+          <t>Values</t>
         </is>
       </c>
       <c r="F190" s="12" t="n"/>
@@ -7354,7 +7349,7 @@
       <c r="J190" s="12" t="n"/>
       <c r="K190" s="12" t="inlineStr">
         <is>
-          <t>dataUrl</t>
+          <t>values</t>
         </is>
       </c>
       <c r="L190" s="12" t="n"/>
@@ -7371,12 +7366,12 @@
       <c r="C191" s="12" t="inlineStr"/>
       <c r="D191" s="12" t="inlineStr">
         <is>
-          <t>valuesField</t>
+          <t>onChangeField</t>
         </is>
       </c>
       <c r="E191" s="12" t="inlineStr">
         <is>
-          <t>Values</t>
+          <t>On Change</t>
         </is>
       </c>
       <c r="F191" s="12" t="n"/>
@@ -7390,7 +7385,7 @@
       <c r="J191" s="12" t="n"/>
       <c r="K191" s="12" t="inlineStr">
         <is>
-          <t>values</t>
+          <t>onChange</t>
         </is>
       </c>
       <c r="L191" s="12" t="n"/>
@@ -7407,12 +7402,12 @@
       <c r="C192" s="12" t="inlineStr"/>
       <c r="D192" s="12" t="inlineStr">
         <is>
-          <t>onChangeField</t>
+          <t>dialogField</t>
         </is>
       </c>
       <c r="E192" s="12" t="inlineStr">
         <is>
-          <t>On Change</t>
+          <t>Dialog</t>
         </is>
       </c>
       <c r="F192" s="12" t="n"/>
@@ -7420,13 +7415,13 @@
       <c r="H192" s="12" t="inlineStr"/>
       <c r="I192" s="12" t="inlineStr">
         <is>
-          <t>TextBox</t>
+          <t>TextArea</t>
         </is>
       </c>
       <c r="J192" s="12" t="n"/>
       <c r="K192" s="12" t="inlineStr">
         <is>
-          <t>onChange</t>
+          <t>dialog</t>
         </is>
       </c>
       <c r="L192" s="12" t="n"/>
@@ -7434,283 +7429,247 @@
       <c r="N192" s="12" t="n"/>
       <c r="O192" s="12" t="inlineStr">
         <is>
-          <t>width: 255px;</t>
+          <t>width: 256px;</t>
         </is>
       </c>
       <c r="P192" s="12" t="n"/>
     </row>
     <row r="193">
-      <c r="C193" s="12" t="inlineStr"/>
-      <c r="D193" s="12" t="inlineStr">
-        <is>
-          <t>dialogField</t>
-        </is>
-      </c>
-      <c r="E193" s="12" t="inlineStr">
-        <is>
-          <t>Dialog</t>
-        </is>
-      </c>
-      <c r="F193" s="12" t="n"/>
-      <c r="G193" s="12" t="inlineStr"/>
-      <c r="H193" s="12" t="inlineStr"/>
-      <c r="I193" s="12" t="inlineStr">
-        <is>
-          <t>TextArea</t>
-        </is>
-      </c>
-      <c r="J193" s="12" t="n"/>
-      <c r="K193" s="12" t="inlineStr">
-        <is>
-          <t>dialog</t>
-        </is>
-      </c>
-      <c r="L193" s="12" t="n"/>
-      <c r="M193" s="12" t="n"/>
-      <c r="N193" s="12" t="n"/>
-      <c r="O193" s="12" t="inlineStr">
-        <is>
-          <t>width: 256px;</t>
-        </is>
-      </c>
-      <c r="P193" s="12" t="n"/>
-    </row>
-    <row r="194">
-      <c r="C194" s="5" t="inlineStr">
+      <c r="C193" s="5" t="inlineStr">
         <is>
           <t>End of Table</t>
         </is>
       </c>
-      <c r="D194" s="3" t="n"/>
-      <c r="E194" s="3" t="n"/>
-      <c r="F194" s="3" t="n"/>
-      <c r="G194" s="3" t="n"/>
-      <c r="H194" s="3" t="n"/>
-      <c r="I194" s="3" t="n"/>
-      <c r="J194" s="3" t="n"/>
-      <c r="K194" s="3" t="n"/>
-      <c r="L194" s="3" t="n"/>
-      <c r="M194" s="3" t="n"/>
-      <c r="N194" s="3" t="n"/>
-      <c r="O194" s="3" t="n"/>
-      <c r="P194" s="3" t="n"/>
-    </row>
+      <c r="D193" s="3" t="n"/>
+      <c r="E193" s="3" t="n"/>
+      <c r="F193" s="3" t="n"/>
+      <c r="G193" s="3" t="n"/>
+      <c r="H193" s="3" t="n"/>
+      <c r="I193" s="3" t="n"/>
+      <c r="J193" s="3" t="n"/>
+      <c r="K193" s="3" t="n"/>
+      <c r="L193" s="3" t="n"/>
+      <c r="M193" s="3" t="n"/>
+      <c r="N193" s="3" t="n"/>
+      <c r="O193" s="3" t="n"/>
+      <c r="P193" s="3" t="n"/>
+    </row>
+    <row r="194"/>
     <row r="195"/>
     <row r="196"/>
-    <row r="197"/>
+    <row r="197">
+      <c r="A197" s="7" t="inlineStr">
+        <is>
+          <t>subScreenTable</t>
+        </is>
+      </c>
+      <c r="B197" s="1" t="inlineStr">
+        <is>
+          <t>Sub Screen</t>
+        </is>
+      </c>
+      <c r="C197" s="3" t="inlineStr">
+        <is>
+          <t>Sub Screen Name</t>
+        </is>
+      </c>
+      <c r="D197" s="3" t="inlineStr">
+        <is>
+          <t>Field Groups</t>
+        </is>
+      </c>
+      <c r="E197" s="3" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
+      </c>
+    </row>
     <row r="198">
-      <c r="A198" s="7" t="inlineStr">
-        <is>
-          <t>subScreenTable</t>
-        </is>
-      </c>
-      <c r="B198" s="1" t="inlineStr">
-        <is>
-          <t>Sub Screen</t>
-        </is>
-      </c>
-      <c r="C198" s="3" t="inlineStr">
-        <is>
-          <t>Sub Screen Name</t>
-        </is>
-      </c>
-      <c r="D198" s="3" t="inlineStr">
-        <is>
-          <t>Field Groups</t>
-        </is>
-      </c>
-      <c r="E198" s="3" t="inlineStr">
-        <is>
-          <t>Remarks</t>
-        </is>
-      </c>
+      <c r="C198" s="12" t="inlineStr">
+        <is>
+          <t>Main Screen</t>
+        </is>
+      </c>
+      <c r="D198" s="12" t="inlineStr">
+        <is>
+          <t>fgHeaderFooterDtlFg, fgHeaderFooterListFg, fgHeaderFooterToolbar, fgLinkDtlFg, fgLinkListFg, fgLinkToolbar, fgToolbar, fieldGroupDtlFg, fieldGroupListFg, fieldListFg, importFg, recordsetListFg, recordsetToolbar, screenDtlFg, screenSelectionFg, screenToolbar1, screenToolbar2, subScreenFg, subScreenToolbar</t>
+        </is>
+      </c>
+      <c r="E198" s="12" t="n"/>
     </row>
     <row r="199">
       <c r="C199" s="12" t="inlineStr">
         <is>
-          <t>Main Screen</t>
+          <t>widgetPramsDialog</t>
         </is>
       </c>
       <c r="D199" s="12" t="inlineStr">
         <is>
-          <t>fgHeaderFooterDtlFg, fgHeaderFooterListFg, fgHeaderFooterToolbar, fgLinkDtlFg, fgLinkListFg, fgLinkToolbar, fgToolbar, fieldGroupDtlFg, fieldGroupListFg, fieldListFg, importFg, recordsetListFg, recordsetToolbar, screenDtlFg, screenSelectionFg, screenToolbar1, screenToolbar2, subScreenFg, subScreenToolbar</t>
+          <t>dialogWidgetPramsFg, dialogHtml</t>
         </is>
       </c>
       <c r="E199" s="12" t="n"/>
     </row>
     <row r="200">
-      <c r="C200" s="12" t="inlineStr">
-        <is>
-          <t>widgetPramsDialog</t>
-        </is>
-      </c>
-      <c r="D200" s="12" t="inlineStr">
-        <is>
-          <t>dialogWidgetPramsFg, dialogHtml</t>
-        </is>
-      </c>
-      <c r="E200" s="12" t="n"/>
-    </row>
-    <row r="201">
-      <c r="C201" s="5" t="inlineStr">
+      <c r="C200" s="5" t="inlineStr">
         <is>
           <t>End of Table</t>
         </is>
       </c>
-      <c r="D201" s="3" t="n"/>
-      <c r="E201" s="3" t="n"/>
-    </row>
+      <c r="D200" s="3" t="n"/>
+      <c r="E200" s="3" t="n"/>
+    </row>
+    <row r="201"/>
     <row r="202"/>
-    <row r="203"/>
+    <row r="203">
+      <c r="B203" s="1" t="n"/>
+    </row>
     <row r="204">
-      <c r="B204" s="1" t="n"/>
+      <c r="A204" s="7" t="inlineStr">
+        <is>
+          <t>fieldGroupLinkTable</t>
+        </is>
+      </c>
+      <c r="B204" s="1" t="inlineStr">
+        <is>
+          <t>Field Group Links</t>
+        </is>
+      </c>
+      <c r="C204" s="3" t="inlineStr">
+        <is>
+          <t>Field Group Name</t>
+        </is>
+      </c>
+      <c r="D204" s="3" t="inlineStr">
+        <is>
+          <t>Local Key</t>
+        </is>
+      </c>
+      <c r="E204" s="3" t="inlineStr">
+        <is>
+          <t>Parent Field Group Name</t>
+        </is>
+      </c>
+      <c r="F204" s="3" t="inlineStr">
+        <is>
+          <t>Parent Key</t>
+        </is>
+      </c>
+      <c r="G204" s="3" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
+      </c>
     </row>
     <row r="205">
-      <c r="A205" s="7" t="inlineStr">
-        <is>
-          <t>fieldGroupLinkTable</t>
-        </is>
-      </c>
-      <c r="B205" s="1" t="inlineStr">
-        <is>
-          <t>Field Group Links</t>
-        </is>
-      </c>
-      <c r="C205" s="3" t="inlineStr">
+      <c r="C205" s="12" t="n"/>
+      <c r="D205" s="12" t="n"/>
+      <c r="E205" s="12" t="n"/>
+      <c r="F205" s="12" t="n"/>
+      <c r="G205" s="12" t="n"/>
+    </row>
+    <row r="206">
+      <c r="C206" s="5" t="inlineStr">
+        <is>
+          <t>End of Table</t>
+        </is>
+      </c>
+      <c r="D206" s="3" t="n"/>
+      <c r="E206" s="3" t="n"/>
+      <c r="F206" s="3" t="n"/>
+      <c r="G206" s="3" t="n"/>
+    </row>
+    <row r="207"/>
+    <row r="208"/>
+    <row r="209">
+      <c r="B209" s="18" t="inlineStr">
+        <is>
+          <t>Table Header and Footer for Field Groups</t>
+        </is>
+      </c>
+      <c r="E209" s="8" t="inlineStr">
+        <is>
+          <t>add as many levels as needed</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="14" t="inlineStr">
+        <is>
+          <t>headerFooterTable</t>
+        </is>
+      </c>
+      <c r="B210" s="15" t="n"/>
+      <c r="C210" s="19" t="inlineStr">
         <is>
           <t>Field Group Name</t>
         </is>
       </c>
-      <c r="D205" s="3" t="inlineStr">
-        <is>
-          <t>Local Key</t>
-        </is>
-      </c>
-      <c r="E205" s="3" t="inlineStr">
-        <is>
-          <t>Parent Field Group Name</t>
-        </is>
-      </c>
-      <c r="F205" s="3" t="inlineStr">
-        <is>
-          <t>Parent Key</t>
-        </is>
-      </c>
-      <c r="G205" s="3" t="inlineStr">
+      <c r="D210" s="19" t="inlineStr">
+        <is>
+          <t>Field</t>
+        </is>
+      </c>
+      <c r="E210" s="19" t="inlineStr">
+        <is>
+          <t>Header Level 1</t>
+        </is>
+      </c>
+      <c r="F210" s="19" t="inlineStr">
+        <is>
+          <t>Header Level 2</t>
+        </is>
+      </c>
+      <c r="G210" s="19" t="inlineStr">
+        <is>
+          <t>Header Level 3</t>
+        </is>
+      </c>
+      <c r="H210" s="19" t="inlineStr">
+        <is>
+          <t>Footer</t>
+        </is>
+      </c>
+      <c r="I210" s="19" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
-    </row>
-    <row r="206">
-      <c r="C206" s="12" t="n"/>
-      <c r="D206" s="12" t="n"/>
-      <c r="E206" s="12" t="n"/>
-      <c r="F206" s="12" t="n"/>
-      <c r="G206" s="12" t="n"/>
-    </row>
-    <row r="207">
-      <c r="C207" s="5" t="inlineStr">
+      <c r="K210" s="8" t="inlineStr">
+        <is>
+          <t>optional for table field groups only</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="C211" s="12" t="n"/>
+      <c r="D211" s="12" t="n"/>
+      <c r="E211" s="12" t="n"/>
+      <c r="F211" s="12" t="n"/>
+      <c r="G211" s="12" t="n"/>
+      <c r="H211" s="12" t="n"/>
+      <c r="I211" s="12" t="n"/>
+      <c r="K211" s="8" t="inlineStr">
+        <is>
+          <t>this is only an example, does not match the above definition</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="C212" s="5" t="inlineStr">
         <is>
           <t>End of Table</t>
         </is>
       </c>
-      <c r="D207" s="3" t="n"/>
-      <c r="E207" s="3" t="n"/>
-      <c r="F207" s="3" t="n"/>
-      <c r="G207" s="3" t="n"/>
-    </row>
-    <row r="208"/>
-    <row r="209"/>
-    <row r="210">
-      <c r="B210" s="18" t="inlineStr">
-        <is>
-          <t>Table Header and Footer for Field Groups</t>
-        </is>
-      </c>
-      <c r="E210" s="8" t="inlineStr">
-        <is>
-          <t>add as many levels as needed</t>
-        </is>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" s="14" t="inlineStr">
-        <is>
-          <t>headerFooterTable</t>
-        </is>
-      </c>
-      <c r="B211" s="15" t="n"/>
-      <c r="C211" s="19" t="inlineStr">
-        <is>
-          <t>Field Group Name</t>
-        </is>
-      </c>
-      <c r="D211" s="19" t="inlineStr">
-        <is>
-          <t>Field</t>
-        </is>
-      </c>
-      <c r="E211" s="19" t="inlineStr">
-        <is>
-          <t>Header Level 1</t>
-        </is>
-      </c>
-      <c r="F211" s="19" t="inlineStr">
-        <is>
-          <t>Header Level 2</t>
-        </is>
-      </c>
-      <c r="G211" s="19" t="inlineStr">
-        <is>
-          <t>Header Level 3</t>
-        </is>
-      </c>
-      <c r="H211" s="19" t="inlineStr">
-        <is>
-          <t>Footer</t>
-        </is>
-      </c>
-      <c r="I211" s="19" t="inlineStr">
-        <is>
-          <t>Remarks</t>
-        </is>
-      </c>
-      <c r="K211" s="8" t="inlineStr">
-        <is>
-          <t>optional for table field groups only</t>
-        </is>
-      </c>
-    </row>
-    <row r="212">
-      <c r="C212" s="12" t="n"/>
-      <c r="D212" s="12" t="n"/>
-      <c r="E212" s="12" t="n"/>
-      <c r="F212" s="12" t="n"/>
-      <c r="G212" s="12" t="n"/>
-      <c r="H212" s="12" t="n"/>
-      <c r="I212" s="12" t="n"/>
-      <c r="K212" s="8" t="inlineStr">
-        <is>
-          <t>this is only an example, does not match the above definition</t>
-        </is>
-      </c>
+      <c r="D212" s="3" t="n"/>
+      <c r="E212" s="3" t="n"/>
+      <c r="F212" s="3" t="n"/>
+      <c r="G212" s="3" t="n"/>
+      <c r="H212" s="3" t="n"/>
+      <c r="I212" s="3" t="n"/>
     </row>
     <row r="213">
-      <c r="C213" s="5" t="inlineStr">
-        <is>
-          <t>End of Table</t>
-        </is>
-      </c>
-      <c r="D213" s="3" t="n"/>
-      <c r="E213" s="3" t="n"/>
-      <c r="F213" s="3" t="n"/>
-      <c r="G213" s="3" t="n"/>
-      <c r="H213" s="3" t="n"/>
-      <c r="I213" s="3" t="n"/>
-    </row>
-    <row r="214">
-      <c r="H214" s="8" t="n"/>
+      <c r="H213" s="8" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>